<commit_message>
charts and parser generated sources
</commit_message>
<xml_diff>
--- a/src/main/resources/outputs/f5_d1.xlsx
+++ b/src/main/resources/outputs/f5_d1.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdjur\Documents\Programowanie\Intellij\Programowanie Genetyczne\tinyGPDataGenerator\src\main\resources\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831972D9-46E4-4DA1-A499-E1E3B05E51E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA4D095-BF23-481E-A32D-6CCFC7922D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="f5_d1" sheetId="1" r:id="rId1"/>
     <sheet name="Evaluation Warning" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -16578,3161 +16575,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="f6_d4"/>
-      <sheetName val="Evaluation Warning"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="I3" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="J3">
-            <v>3694773.23398316</v>
-          </cell>
-          <cell r="K3">
-            <v>3390545.46796632</v>
-          </cell>
-          <cell r="L3">
-            <v>3094317.70194948</v>
-          </cell>
-          <cell r="M3">
-            <v>2806089.93593264</v>
-          </cell>
-          <cell r="N3">
-            <v>2525862.1699158102</v>
-          </cell>
-          <cell r="O3">
-            <v>2253634.4038989702</v>
-          </cell>
-          <cell r="P3">
-            <v>1989406.63788213</v>
-          </cell>
-          <cell r="Q3">
-            <v>1733178.87186529</v>
-          </cell>
-          <cell r="R3">
-            <v>1484951.10584846</v>
-          </cell>
-          <cell r="S3">
-            <v>1244723.33983162</v>
-          </cell>
-          <cell r="T3">
-            <v>1012495.57381478</v>
-          </cell>
-          <cell r="U3">
-            <v>788267.80779794499</v>
-          </cell>
-          <cell r="V3">
-            <v>572040.04178110696</v>
-          </cell>
-          <cell r="W3">
-            <v>363812.275764269</v>
-          </cell>
-          <cell r="X3">
-            <v>163584.50974743199</v>
-          </cell>
-          <cell r="Y3">
-            <v>-28643.256269405902</v>
-          </cell>
-          <cell r="Z3">
-            <v>-212871.02228624301</v>
-          </cell>
-          <cell r="AA3">
-            <v>-389098.788303081</v>
-          </cell>
-          <cell r="AB3">
-            <v>-557326.55431991897</v>
-          </cell>
-          <cell r="AC3">
-            <v>-717554.32033675699</v>
-          </cell>
-          <cell r="AD3">
-            <v>-869782.08635359502</v>
-          </cell>
-          <cell r="AE3">
-            <v>-1014009.85237043</v>
-          </cell>
-          <cell r="AF3">
-            <v>-1150237.61838727</v>
-          </cell>
-          <cell r="AG3">
-            <v>-1278465.3844041</v>
-          </cell>
-          <cell r="AH3">
-            <v>-1398693.15042094</v>
-          </cell>
-          <cell r="AI3">
-            <v>-1510920.91643778</v>
-          </cell>
-          <cell r="AJ3">
-            <v>-1615148.68245462</v>
-          </cell>
-          <cell r="AK3">
-            <v>-1711376.44847146</v>
-          </cell>
-          <cell r="AL3">
-            <v>-1799604.21448829</v>
-          </cell>
-          <cell r="AM3">
-            <v>-1879831.98050513</v>
-          </cell>
-          <cell r="AN3">
-            <v>-1952059.74652197</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="I4">
-            <v>3816821.6215174701</v>
-          </cell>
-          <cell r="J4">
-            <v>3516593.8555006301</v>
-          </cell>
-          <cell r="K4">
-            <v>3224366.0894837901</v>
-          </cell>
-          <cell r="L4">
-            <v>2940138.3234669599</v>
-          </cell>
-          <cell r="M4">
-            <v>2663910.5574501199</v>
-          </cell>
-          <cell r="N4">
-            <v>2395682.7914332799</v>
-          </cell>
-          <cell r="O4">
-            <v>2135455.0254164399</v>
-          </cell>
-          <cell r="P4">
-            <v>1883227.2593996001</v>
-          </cell>
-          <cell r="Q4">
-            <v>1638999.4933827701</v>
-          </cell>
-          <cell r="R4">
-            <v>1402771.7273659301</v>
-          </cell>
-          <cell r="S4">
-            <v>1174543.9613490901</v>
-          </cell>
-          <cell r="T4">
-            <v>954316.19533225696</v>
-          </cell>
-          <cell r="U4">
-            <v>742088.42931541905</v>
-          </cell>
-          <cell r="V4">
-            <v>537860.66329858103</v>
-          </cell>
-          <cell r="W4">
-            <v>341632.897281743</v>
-          </cell>
-          <cell r="X4">
-            <v>153405.13126490501</v>
-          </cell>
-          <cell r="Y4">
-            <v>-26822.634751932299</v>
-          </cell>
-          <cell r="Z4">
-            <v>-199050.40076876999</v>
-          </cell>
-          <cell r="AA4">
-            <v>-363278.16678560799</v>
-          </cell>
-          <cell r="AB4">
-            <v>-519505.93280244601</v>
-          </cell>
-          <cell r="AC4">
-            <v>-667733.69881928398</v>
-          </cell>
-          <cell r="AD4">
-            <v>-807961.464836122</v>
-          </cell>
-          <cell r="AE4">
-            <v>-940189.23085295898</v>
-          </cell>
-          <cell r="AF4">
-            <v>-1064416.9968697899</v>
-          </cell>
-          <cell r="AG4">
-            <v>-1180644.7628866299</v>
-          </cell>
-          <cell r="AH4">
-            <v>-1288872.5289034699</v>
-          </cell>
-          <cell r="AI4">
-            <v>-1389100.2949203099</v>
-          </cell>
-          <cell r="AJ4">
-            <v>-1481328.0609371399</v>
-          </cell>
-          <cell r="AK4">
-            <v>-1565555.8269539799</v>
-          </cell>
-          <cell r="AL4">
-            <v>-1641783.5929708199</v>
-          </cell>
-          <cell r="AM4">
-            <v>-1710011.3589876599</v>
-          </cell>
-          <cell r="AN4">
-            <v>-1770239.1250044999</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="I5">
-            <v>4007001</v>
-          </cell>
-          <cell r="J5">
-            <v>3338414.47701811</v>
-          </cell>
-          <cell r="K5">
-            <v>3058186.71100127</v>
-          </cell>
-          <cell r="L5">
-            <v>2785958.94498443</v>
-          </cell>
-          <cell r="M5">
-            <v>2521731.17896759</v>
-          </cell>
-          <cell r="N5">
-            <v>2265503.41295075</v>
-          </cell>
-          <cell r="O5">
-            <v>2017275.64693392</v>
-          </cell>
-          <cell r="P5">
-            <v>1777047.88091708</v>
-          </cell>
-          <cell r="Q5">
-            <v>1544820.11490024</v>
-          </cell>
-          <cell r="R5">
-            <v>1320592.3488834</v>
-          </cell>
-          <cell r="S5">
-            <v>1104364.58286656</v>
-          </cell>
-          <cell r="T5">
-            <v>896136.81684973103</v>
-          </cell>
-          <cell r="U5">
-            <v>695909.050832893</v>
-          </cell>
-          <cell r="V5">
-            <v>503681.28481605498</v>
-          </cell>
-          <cell r="W5">
-            <v>319453.51879921701</v>
-          </cell>
-          <cell r="X5">
-            <v>143225.75278237899</v>
-          </cell>
-          <cell r="Y5">
-            <v>-25002.0132344587</v>
-          </cell>
-          <cell r="Z5">
-            <v>-185229.77925129599</v>
-          </cell>
-          <cell r="AA5">
-            <v>-337457.54526813398</v>
-          </cell>
-          <cell r="AB5">
-            <v>-481685.31128497201</v>
-          </cell>
-          <cell r="AC5">
-            <v>-617913.07730181003</v>
-          </cell>
-          <cell r="AD5">
-            <v>-746140.84331864805</v>
-          </cell>
-          <cell r="AE5">
-            <v>-866368.60933548596</v>
-          </cell>
-          <cell r="AF5">
-            <v>-978596.37535232399</v>
-          </cell>
-          <cell r="AG5">
-            <v>-1082824.14136916</v>
-          </cell>
-          <cell r="AH5">
-            <v>-1179051.907386</v>
-          </cell>
-          <cell r="AI5">
-            <v>-1267279.67340283</v>
-          </cell>
-          <cell r="AJ5">
-            <v>-1347507.43941967</v>
-          </cell>
-          <cell r="AK5">
-            <v>-1419735.20543651</v>
-          </cell>
-          <cell r="AL5">
-            <v>-1483962.97145335</v>
-          </cell>
-          <cell r="AM5">
-            <v>-1540190.73747019</v>
-          </cell>
-          <cell r="AN5">
-            <v>-1588418.50348702</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="I6">
-            <v>3436462.8645524201</v>
-          </cell>
-          <cell r="J6">
-            <v>3160235.0985355801</v>
-          </cell>
-          <cell r="K6">
-            <v>2892007.3325187401</v>
-          </cell>
-          <cell r="L6">
-            <v>2631779.5665019001</v>
-          </cell>
-          <cell r="M6">
-            <v>2379551.8004850699</v>
-          </cell>
-          <cell r="N6">
-            <v>2135324.0344682299</v>
-          </cell>
-          <cell r="O6">
-            <v>1899096.2684513901</v>
-          </cell>
-          <cell r="P6">
-            <v>1670868.5024345501</v>
-          </cell>
-          <cell r="Q6">
-            <v>1450640.7364177101</v>
-          </cell>
-          <cell r="R6">
-            <v>1238412.9704008801</v>
-          </cell>
-          <cell r="S6">
-            <v>1034185.20438404</v>
-          </cell>
-          <cell r="T6">
-            <v>837957.43836720497</v>
-          </cell>
-          <cell r="U6">
-            <v>649729.67235036695</v>
-          </cell>
-          <cell r="V6">
-            <v>469501.90633352799</v>
-          </cell>
-          <cell r="W6">
-            <v>297274.14031669003</v>
-          </cell>
-          <cell r="X6">
-            <v>133046.374299852</v>
-          </cell>
-          <cell r="Y6">
-            <v>-23181.391716985101</v>
-          </cell>
-          <cell r="Z6">
-            <v>-171409.157733823</v>
-          </cell>
-          <cell r="AA6">
-            <v>-311636.92375066102</v>
-          </cell>
-          <cell r="AB6">
-            <v>-443864.68976749899</v>
-          </cell>
-          <cell r="AC6">
-            <v>-568092.45578433701</v>
-          </cell>
-          <cell r="AD6">
-            <v>-684320.22180117504</v>
-          </cell>
-          <cell r="AE6">
-            <v>-792547.98781801295</v>
-          </cell>
-          <cell r="AF6">
-            <v>-892775.75383485097</v>
-          </cell>
-          <cell r="AG6">
-            <v>-985003.51985168899</v>
-          </cell>
-          <cell r="AH6">
-            <v>-1069231.2858685199</v>
-          </cell>
-          <cell r="AI6">
-            <v>-1145459.0518853599</v>
-          </cell>
-          <cell r="AJ6">
-            <v>-1213686.8179021999</v>
-          </cell>
-          <cell r="AK6">
-            <v>-1273914.5839190399</v>
-          </cell>
-          <cell r="AL6">
-            <v>-1326142.3499358699</v>
-          </cell>
-          <cell r="AM6">
-            <v>-1370370.1159527099</v>
-          </cell>
-          <cell r="AN6">
-            <v>-1406597.8819695499</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="I7">
-            <v>3246283.4860698902</v>
-          </cell>
-          <cell r="J7">
-            <v>2982055.7200530502</v>
-          </cell>
-          <cell r="K7">
-            <v>2725827.95403622</v>
-          </cell>
-          <cell r="L7">
-            <v>2477600.18801938</v>
-          </cell>
-          <cell r="M7">
-            <v>2237372.42200254</v>
-          </cell>
-          <cell r="N7">
-            <v>2005144.6559857</v>
-          </cell>
-          <cell r="O7">
-            <v>1780916.88996886</v>
-          </cell>
-          <cell r="P7">
-            <v>1564689.12395203</v>
-          </cell>
-          <cell r="Q7">
-            <v>1356461.35793519</v>
-          </cell>
-          <cell r="R7">
-            <v>1156233.59191835</v>
-          </cell>
-          <cell r="S7">
-            <v>964005.82590151601</v>
-          </cell>
-          <cell r="T7">
-            <v>779778.05988467799</v>
-          </cell>
-          <cell r="U7">
-            <v>603550.29386783997</v>
-          </cell>
-          <cell r="V7">
-            <v>435322.527851002</v>
-          </cell>
-          <cell r="W7">
-            <v>275094.76183416398</v>
-          </cell>
-          <cell r="X7">
-            <v>122866.99581732599</v>
-          </cell>
-          <cell r="Y7">
-            <v>-21360.770199511499</v>
-          </cell>
-          <cell r="Z7">
-            <v>-157588.53621634899</v>
-          </cell>
-          <cell r="AA7">
-            <v>-285816.30223318702</v>
-          </cell>
-          <cell r="AB7">
-            <v>-406044.06825002498</v>
-          </cell>
-          <cell r="AC7">
-            <v>-518271.83426686301</v>
-          </cell>
-          <cell r="AD7">
-            <v>-622499.60028370097</v>
-          </cell>
-          <cell r="AE7">
-            <v>-718727.366300539</v>
-          </cell>
-          <cell r="AF7">
-            <v>-806955.13231737702</v>
-          </cell>
-          <cell r="AG7">
-            <v>-887182.89833421505</v>
-          </cell>
-          <cell r="AH7">
-            <v>-959410.66435105295</v>
-          </cell>
-          <cell r="AI7">
-            <v>-1023638.43036789</v>
-          </cell>
-          <cell r="AJ7">
-            <v>-1079866.19638472</v>
-          </cell>
-          <cell r="AK7">
-            <v>-1128093.96240156</v>
-          </cell>
-          <cell r="AL7">
-            <v>-1168321.7284184</v>
-          </cell>
-          <cell r="AM7">
-            <v>-1200549.49443524</v>
-          </cell>
-          <cell r="AN7">
-            <v>-1224777.2604520801</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="I8">
-            <v>3056104.1075873598</v>
-          </cell>
-          <cell r="J8">
-            <v>2803876.3415705301</v>
-          </cell>
-          <cell r="K8">
-            <v>2559648.5755536901</v>
-          </cell>
-          <cell r="L8">
-            <v>2323420.8095368501</v>
-          </cell>
-          <cell r="M8">
-            <v>2095193.0435200101</v>
-          </cell>
-          <cell r="N8">
-            <v>1874965.2775031701</v>
-          </cell>
-          <cell r="O8">
-            <v>1662737.5114863401</v>
-          </cell>
-          <cell r="P8">
-            <v>1458509.7454695001</v>
-          </cell>
-          <cell r="Q8">
-            <v>1262281.9794526601</v>
-          </cell>
-          <cell r="R8">
-            <v>1074054.2134358201</v>
-          </cell>
-          <cell r="S8">
-            <v>893826.44741898996</v>
-          </cell>
-          <cell r="T8">
-            <v>721598.68140215205</v>
-          </cell>
-          <cell r="U8">
-            <v>557370.91538531403</v>
-          </cell>
-          <cell r="V8">
-            <v>401143.14936847601</v>
-          </cell>
-          <cell r="W8">
-            <v>252915.38335163801</v>
-          </cell>
-          <cell r="X8">
-            <v>112687.6173348</v>
-          </cell>
-          <cell r="Y8">
-            <v>-19540.1486820379</v>
-          </cell>
-          <cell r="Z8">
-            <v>-143767.91469887501</v>
-          </cell>
-          <cell r="AA8">
-            <v>-259995.680715714</v>
-          </cell>
-          <cell r="AB8">
-            <v>-368223.44673255202</v>
-          </cell>
-          <cell r="AC8">
-            <v>-468451.21274938999</v>
-          </cell>
-          <cell r="AD8">
-            <v>-560678.97876622796</v>
-          </cell>
-          <cell r="AE8">
-            <v>-644906.74478306598</v>
-          </cell>
-          <cell r="AF8">
-            <v>-721134.510799904</v>
-          </cell>
-          <cell r="AG8">
-            <v>-789362.27681674203</v>
-          </cell>
-          <cell r="AH8">
-            <v>-849590.04283358005</v>
-          </cell>
-          <cell r="AI8">
-            <v>-901817.80885041796</v>
-          </cell>
-          <cell r="AJ8">
-            <v>-946045.57486725505</v>
-          </cell>
-          <cell r="AK8">
-            <v>-982273.34088409401</v>
-          </cell>
-          <cell r="AL8">
-            <v>-1010501.1069009301</v>
-          </cell>
-          <cell r="AM8">
-            <v>-1030728.8729177699</v>
-          </cell>
-          <cell r="AN8">
-            <v>-1042956.6389346001</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="I9">
-            <v>2865924.7291048402</v>
-          </cell>
-          <cell r="J9">
-            <v>2625696.9630880002</v>
-          </cell>
-          <cell r="K9">
-            <v>2393469.1970711602</v>
-          </cell>
-          <cell r="L9">
-            <v>2169241.4310543202</v>
-          </cell>
-          <cell r="M9">
-            <v>1953013.66503749</v>
-          </cell>
-          <cell r="N9">
-            <v>1744785.89902065</v>
-          </cell>
-          <cell r="O9">
-            <v>1544558.13300381</v>
-          </cell>
-          <cell r="P9">
-            <v>1352330.36698697</v>
-          </cell>
-          <cell r="Q9">
-            <v>1168102.60097014</v>
-          </cell>
-          <cell r="R9">
-            <v>991874.83495330205</v>
-          </cell>
-          <cell r="S9">
-            <v>823647.06893646298</v>
-          </cell>
-          <cell r="T9">
-            <v>663419.30291962496</v>
-          </cell>
-          <cell r="U9">
-            <v>511191.53690278699</v>
-          </cell>
-          <cell r="V9">
-            <v>366963.77088594902</v>
-          </cell>
-          <cell r="W9">
-            <v>230736.004869111</v>
-          </cell>
-          <cell r="X9">
-            <v>102508.238852273</v>
-          </cell>
-          <cell r="Y9">
-            <v>-17719.527164564301</v>
-          </cell>
-          <cell r="Z9">
-            <v>-129947.293181402</v>
-          </cell>
-          <cell r="AA9">
-            <v>-234175.05919823999</v>
-          </cell>
-          <cell r="AB9">
-            <v>-330402.82521507802</v>
-          </cell>
-          <cell r="AC9">
-            <v>-418630.59123191598</v>
-          </cell>
-          <cell r="AD9">
-            <v>-498858.35724875401</v>
-          </cell>
-          <cell r="AE9">
-            <v>-571086.12326559203</v>
-          </cell>
-          <cell r="AF9">
-            <v>-635313.88928243006</v>
-          </cell>
-          <cell r="AG9">
-            <v>-691541.65529926796</v>
-          </cell>
-          <cell r="AH9">
-            <v>-739769.42131610599</v>
-          </cell>
-          <cell r="AI9">
-            <v>-779997.18733294401</v>
-          </cell>
-          <cell r="AJ9">
-            <v>-812224.95334978204</v>
-          </cell>
-          <cell r="AK9">
-            <v>-836452.71936661995</v>
-          </cell>
-          <cell r="AL9">
-            <v>-852680.48538345902</v>
-          </cell>
-          <cell r="AM9">
-            <v>-860908.25140029599</v>
-          </cell>
-          <cell r="AN9">
-            <v>-861136.01741713402</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="I10">
-            <v>2675745.3506223098</v>
-          </cell>
-          <cell r="J10">
-            <v>2447517.5846054698</v>
-          </cell>
-          <cell r="K10">
-            <v>2227289.8185886401</v>
-          </cell>
-          <cell r="L10">
-            <v>2015062.0525718001</v>
-          </cell>
-          <cell r="M10">
-            <v>1810834.2865549601</v>
-          </cell>
-          <cell r="N10">
-            <v>1614606.5205381201</v>
-          </cell>
-          <cell r="O10">
-            <v>1426378.7545212801</v>
-          </cell>
-          <cell r="P10">
-            <v>1246150.9885044501</v>
-          </cell>
-          <cell r="Q10">
-            <v>1073923.2224876101</v>
-          </cell>
-          <cell r="R10">
-            <v>909695.45647077495</v>
-          </cell>
-          <cell r="S10">
-            <v>753467.69045393704</v>
-          </cell>
-          <cell r="T10">
-            <v>605239.92443709902</v>
-          </cell>
-          <cell r="U10">
-            <v>465012.158420261</v>
-          </cell>
-          <cell r="V10">
-            <v>332784.39240342297</v>
-          </cell>
-          <cell r="W10">
-            <v>208556.62638658501</v>
-          </cell>
-          <cell r="X10">
-            <v>92328.860369747301</v>
-          </cell>
-          <cell r="Y10">
-            <v>-15898.9056470907</v>
-          </cell>
-          <cell r="Z10">
-            <v>-116126.67166392801</v>
-          </cell>
-          <cell r="AA10">
-            <v>-208354.43768076599</v>
-          </cell>
-          <cell r="AB10">
-            <v>-292582.20369760401</v>
-          </cell>
-          <cell r="AC10">
-            <v>-368809.96971444198</v>
-          </cell>
-          <cell r="AD10">
-            <v>-437037.73573128099</v>
-          </cell>
-          <cell r="AE10">
-            <v>-497265.50174811803</v>
-          </cell>
-          <cell r="AF10">
-            <v>-549493.26776495599</v>
-          </cell>
-          <cell r="AG10">
-            <v>-593721.03378179495</v>
-          </cell>
-          <cell r="AH10">
-            <v>-629948.79979863297</v>
-          </cell>
-          <cell r="AI10">
-            <v>-658176.565815471</v>
-          </cell>
-          <cell r="AJ10">
-            <v>-678404.33183230797</v>
-          </cell>
-          <cell r="AK10">
-            <v>-690632.09784914705</v>
-          </cell>
-          <cell r="AL10">
-            <v>-694859.86386598495</v>
-          </cell>
-          <cell r="AM10">
-            <v>-691087.62988282298</v>
-          </cell>
-          <cell r="AN10">
-            <v>-679315.395899661</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="I11">
-            <v>2485565.9721397902</v>
-          </cell>
-          <cell r="J11">
-            <v>2269338.2061229502</v>
-          </cell>
-          <cell r="K11">
-            <v>2061110.4401061099</v>
-          </cell>
-          <cell r="L11">
-            <v>1860882.6740892699</v>
-          </cell>
-          <cell r="M11">
-            <v>1668654.9080724299</v>
-          </cell>
-          <cell r="N11">
-            <v>1484427.1420556</v>
-          </cell>
-          <cell r="O11">
-            <v>1308199.3760387599</v>
-          </cell>
-          <cell r="P11">
-            <v>1139971.6100219199</v>
-          </cell>
-          <cell r="Q11">
-            <v>979743.84400508704</v>
-          </cell>
-          <cell r="R11">
-            <v>827516.07798824902</v>
-          </cell>
-          <cell r="S11">
-            <v>683288.31197141099</v>
-          </cell>
-          <cell r="T11">
-            <v>547060.54595457297</v>
-          </cell>
-          <cell r="U11">
-            <v>418832.779937735</v>
-          </cell>
-          <cell r="V11">
-            <v>298605.01392089698</v>
-          </cell>
-          <cell r="W11">
-            <v>186377.24790405799</v>
-          </cell>
-          <cell r="X11">
-            <v>82149.4818872209</v>
-          </cell>
-          <cell r="Y11">
-            <v>-14078.284129617099</v>
-          </cell>
-          <cell r="Z11">
-            <v>-102306.050146455</v>
-          </cell>
-          <cell r="AA11">
-            <v>-182533.816163293</v>
-          </cell>
-          <cell r="AB11">
-            <v>-254761.58218013099</v>
-          </cell>
-          <cell r="AC11">
-            <v>-318989.34819696902</v>
-          </cell>
-          <cell r="AD11">
-            <v>-375217.11421380698</v>
-          </cell>
-          <cell r="AE11">
-            <v>-423444.88023064501</v>
-          </cell>
-          <cell r="AF11">
-            <v>-463672.64624748298</v>
-          </cell>
-          <cell r="AG11">
-            <v>-495900.412264321</v>
-          </cell>
-          <cell r="AH11">
-            <v>-520128.17828115902</v>
-          </cell>
-          <cell r="AI11">
-            <v>-536355.94429799705</v>
-          </cell>
-          <cell r="AJ11">
-            <v>-544583.71031483496</v>
-          </cell>
-          <cell r="AK11">
-            <v>-544811.47633167298</v>
-          </cell>
-          <cell r="AL11">
-            <v>-537039.242348511</v>
-          </cell>
-          <cell r="AM11">
-            <v>-521267.00836534897</v>
-          </cell>
-          <cell r="AN11">
-            <v>-497494.774382187</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="I12">
-            <v>2295386.5936572598</v>
-          </cell>
-          <cell r="J12">
-            <v>2091158.8276404201</v>
-          </cell>
-          <cell r="K12">
-            <v>1894931.0616235801</v>
-          </cell>
-          <cell r="L12">
-            <v>1706703.2956067501</v>
-          </cell>
-          <cell r="M12">
-            <v>1526475.5295899101</v>
-          </cell>
-          <cell r="N12">
-            <v>1354247.7635730701</v>
-          </cell>
-          <cell r="O12">
-            <v>1190019.9975562301</v>
-          </cell>
-          <cell r="P12">
-            <v>1033792.23153939</v>
-          </cell>
-          <cell r="Q12">
-            <v>885564.46552256006</v>
-          </cell>
-          <cell r="R12">
-            <v>745336.69950572203</v>
-          </cell>
-          <cell r="S12">
-            <v>613108.93348888401</v>
-          </cell>
-          <cell r="T12">
-            <v>488881.16747204599</v>
-          </cell>
-          <cell r="U12">
-            <v>372653.40145520802</v>
-          </cell>
-          <cell r="V12">
-            <v>264425.63543836999</v>
-          </cell>
-          <cell r="W12">
-            <v>164197.869421532</v>
-          </cell>
-          <cell r="X12">
-            <v>71970.103404694499</v>
-          </cell>
-          <cell r="Y12">
-            <v>-12257.6626121435</v>
-          </cell>
-          <cell r="Z12">
-            <v>-88485.428628981506</v>
-          </cell>
-          <cell r="AA12">
-            <v>-156713.19464581899</v>
-          </cell>
-          <cell r="AB12">
-            <v>-216940.96066265699</v>
-          </cell>
-          <cell r="AC12">
-            <v>-269168.72667949501</v>
-          </cell>
-          <cell r="AD12">
-            <v>-313396.49269633298</v>
-          </cell>
-          <cell r="AE12">
-            <v>-349624.258713171</v>
-          </cell>
-          <cell r="AF12">
-            <v>-377852.02473000903</v>
-          </cell>
-          <cell r="AG12">
-            <v>-398079.79074684699</v>
-          </cell>
-          <cell r="AH12">
-            <v>-410307.55676368502</v>
-          </cell>
-          <cell r="AI12">
-            <v>-414535.32278052397</v>
-          </cell>
-          <cell r="AJ12">
-            <v>-410763.08879736101</v>
-          </cell>
-          <cell r="AK12">
-            <v>-398990.85481420002</v>
-          </cell>
-          <cell r="AL12">
-            <v>-379218.62083103799</v>
-          </cell>
-          <cell r="AM12">
-            <v>-351446.38684787601</v>
-          </cell>
-          <cell r="AN12">
-            <v>-315674.15286471398</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="I13">
-            <v>2105207.2151747299</v>
-          </cell>
-          <cell r="J13">
-            <v>1912979.4491578999</v>
-          </cell>
-          <cell r="K13">
-            <v>1728751.6831410599</v>
-          </cell>
-          <cell r="L13">
-            <v>1552523.9171242199</v>
-          </cell>
-          <cell r="M13">
-            <v>1384296.1511073799</v>
-          </cell>
-          <cell r="N13">
-            <v>1224068.3850905399</v>
-          </cell>
-          <cell r="O13">
-            <v>1071840.6190737099</v>
-          </cell>
-          <cell r="P13">
-            <v>927612.85305687203</v>
-          </cell>
-          <cell r="Q13">
-            <v>791385.08704003401</v>
-          </cell>
-          <cell r="R13">
-            <v>663157.32102319598</v>
-          </cell>
-          <cell r="S13">
-            <v>542929.55500635796</v>
-          </cell>
-          <cell r="T13">
-            <v>430701.78898951999</v>
-          </cell>
-          <cell r="U13">
-            <v>326474.02297268203</v>
-          </cell>
-          <cell r="V13">
-            <v>230246.256955844</v>
-          </cell>
-          <cell r="W13">
-            <v>142018.49093900601</v>
-          </cell>
-          <cell r="X13">
-            <v>61790.724922168098</v>
-          </cell>
-          <cell r="Y13">
-            <v>-10437.041094669899</v>
-          </cell>
-          <cell r="Z13">
-            <v>-74664.807111507893</v>
-          </cell>
-          <cell r="AA13">
-            <v>-130892.573128346</v>
-          </cell>
-          <cell r="AB13">
-            <v>-179120.339145184</v>
-          </cell>
-          <cell r="AC13">
-            <v>-219348.105162022</v>
-          </cell>
-          <cell r="AD13">
-            <v>-251575.87117885999</v>
-          </cell>
-          <cell r="AE13">
-            <v>-275803.63719569799</v>
-          </cell>
-          <cell r="AF13">
-            <v>-292031.40321253601</v>
-          </cell>
-          <cell r="AG13">
-            <v>-300259.16922937398</v>
-          </cell>
-          <cell r="AH13">
-            <v>-300486.935246212</v>
-          </cell>
-          <cell r="AI13">
-            <v>-292714.70126305002</v>
-          </cell>
-          <cell r="AJ13">
-            <v>-276942.46727988799</v>
-          </cell>
-          <cell r="AK13">
-            <v>-253170.23329672599</v>
-          </cell>
-          <cell r="AL13">
-            <v>-221397.99931356401</v>
-          </cell>
-          <cell r="AM13">
-            <v>-181625.76533040201</v>
-          </cell>
-          <cell r="AN13">
-            <v>-133853.53134724</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="I14">
-            <v>1915027.8366922101</v>
-          </cell>
-          <cell r="J14">
-            <v>1734800.0706753701</v>
-          </cell>
-          <cell r="K14">
-            <v>1562572.30465853</v>
-          </cell>
-          <cell r="L14">
-            <v>1398344.53864169</v>
-          </cell>
-          <cell r="M14">
-            <v>1242116.77262485</v>
-          </cell>
-          <cell r="N14">
-            <v>1093889.00660802</v>
-          </cell>
-          <cell r="O14">
-            <v>953661.240591184</v>
-          </cell>
-          <cell r="P14">
-            <v>821433.47457434598</v>
-          </cell>
-          <cell r="Q14">
-            <v>697205.70855750795</v>
-          </cell>
-          <cell r="R14">
-            <v>580977.94254067005</v>
-          </cell>
-          <cell r="S14">
-            <v>472750.17652383097</v>
-          </cell>
-          <cell r="T14">
-            <v>372522.41050699301</v>
-          </cell>
-          <cell r="U14">
-            <v>280294.64449015498</v>
-          </cell>
-          <cell r="V14">
-            <v>196066.87847331699</v>
-          </cell>
-          <cell r="W14">
-            <v>119839.11245647899</v>
-          </cell>
-          <cell r="X14">
-            <v>51611.346439641697</v>
-          </cell>
-          <cell r="Y14">
-            <v>-8616.4195771963095</v>
-          </cell>
-          <cell r="Z14">
-            <v>-60844.185594034301</v>
-          </cell>
-          <cell r="AA14">
-            <v>-105071.951610872</v>
-          </cell>
-          <cell r="AB14">
-            <v>-141299.71762770999</v>
-          </cell>
-          <cell r="AC14">
-            <v>-169527.48364454799</v>
-          </cell>
-          <cell r="AD14">
-            <v>-189755.24966138601</v>
-          </cell>
-          <cell r="AE14">
-            <v>-201983.01567822401</v>
-          </cell>
-          <cell r="AF14">
-            <v>-206210.781695062</v>
-          </cell>
-          <cell r="AG14">
-            <v>-202438.5477119</v>
-          </cell>
-          <cell r="AH14">
-            <v>-190666.31372873799</v>
-          </cell>
-          <cell r="AI14">
-            <v>-170894.07974557599</v>
-          </cell>
-          <cell r="AJ14">
-            <v>-143121.84576241401</v>
-          </cell>
-          <cell r="AK14">
-            <v>-107349.61177925199</v>
-          </cell>
-          <cell r="AL14">
-            <v>-63577.377796091103</v>
-          </cell>
-          <cell r="AM14">
-            <v>-11805.143812929</v>
-          </cell>
-          <cell r="AN14">
-            <v>47967.090170232797</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="I15">
-            <v>1724848.4582096799</v>
-          </cell>
-          <cell r="J15">
-            <v>1556620.6921928399</v>
-          </cell>
-          <cell r="K15">
-            <v>1396392.9261759999</v>
-          </cell>
-          <cell r="L15">
-            <v>1244165.1601591699</v>
-          </cell>
-          <cell r="M15">
-            <v>1099937.3941423299</v>
-          </cell>
-          <cell r="N15">
-            <v>963709.62812549504</v>
-          </cell>
-          <cell r="O15">
-            <v>835481.86210865702</v>
-          </cell>
-          <cell r="P15">
-            <v>715254.096091819</v>
-          </cell>
-          <cell r="Q15">
-            <v>603026.33007498097</v>
-          </cell>
-          <cell r="R15">
-            <v>498798.56405814301</v>
-          </cell>
-          <cell r="S15">
-            <v>402570.79804130498</v>
-          </cell>
-          <cell r="T15">
-            <v>314343.03202446701</v>
-          </cell>
-          <cell r="U15">
-            <v>234115.26600762899</v>
-          </cell>
-          <cell r="V15">
-            <v>161887.499990791</v>
-          </cell>
-          <cell r="W15">
-            <v>97659.733973953305</v>
-          </cell>
-          <cell r="X15">
-            <v>41431.967957115303</v>
-          </cell>
-          <cell r="Y15">
-            <v>-6795.7980597227097</v>
-          </cell>
-          <cell r="Z15">
-            <v>-47023.564076560702</v>
-          </cell>
-          <cell r="AA15">
-            <v>-79251.330093398705</v>
-          </cell>
-          <cell r="AB15">
-            <v>-103479.096110236</v>
-          </cell>
-          <cell r="AC15">
-            <v>-119706.862127074</v>
-          </cell>
-          <cell r="AD15">
-            <v>-127934.62814391201</v>
-          </cell>
-          <cell r="AE15">
-            <v>-128162.39416075</v>
-          </cell>
-          <cell r="AF15">
-            <v>-120390.160177588</v>
-          </cell>
-          <cell r="AG15">
-            <v>-104617.92619442601</v>
-          </cell>
-          <cell r="AH15">
-            <v>-80845.692211265006</v>
-          </cell>
-          <cell r="AI15">
-            <v>-49073.458228103002</v>
-          </cell>
-          <cell r="AJ15">
-            <v>-9301.2242449411697</v>
-          </cell>
-          <cell r="AK15">
-            <v>38471.0097382206</v>
-          </cell>
-          <cell r="AL15">
-            <v>94243.243721382401</v>
-          </cell>
-          <cell r="AM15">
-            <v>158015.477704544</v>
-          </cell>
-          <cell r="AN15">
-            <v>229787.711687706</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="I16">
-            <v>1534669.07972715</v>
-          </cell>
-          <cell r="J16">
-            <v>1378441.31371032</v>
-          </cell>
-          <cell r="K16">
-            <v>1230213.54769348</v>
-          </cell>
-          <cell r="L16">
-            <v>1089985.78167664</v>
-          </cell>
-          <cell r="M16">
-            <v>957758.01565980702</v>
-          </cell>
-          <cell r="N16">
-            <v>833530.24964296899</v>
-          </cell>
-          <cell r="O16">
-            <v>717302.48362613097</v>
-          </cell>
-          <cell r="P16">
-            <v>609074.71760929294</v>
-          </cell>
-          <cell r="Q16">
-            <v>508846.95159245498</v>
-          </cell>
-          <cell r="R16">
-            <v>416619.18557561701</v>
-          </cell>
-          <cell r="S16">
-            <v>332391.41955877899</v>
-          </cell>
-          <cell r="T16">
-            <v>256163.65354194099</v>
-          </cell>
-          <cell r="U16">
-            <v>187935.887525103</v>
-          </cell>
-          <cell r="V16">
-            <v>127708.121508265</v>
-          </cell>
-          <cell r="W16">
-            <v>75480.355491426904</v>
-          </cell>
-          <cell r="X16">
-            <v>31252.589474588902</v>
-          </cell>
-          <cell r="Y16">
-            <v>-4975.1765422490998</v>
-          </cell>
-          <cell r="Z16">
-            <v>-33202.942559087103</v>
-          </cell>
-          <cell r="AA16">
-            <v>-53430.708575925099</v>
-          </cell>
-          <cell r="AB16">
-            <v>-65658.474592763203</v>
-          </cell>
-          <cell r="AC16">
-            <v>-69886.240609601198</v>
-          </cell>
-          <cell r="AD16">
-            <v>-66114.006626439295</v>
-          </cell>
-          <cell r="AE16">
-            <v>-54341.772643277298</v>
-          </cell>
-          <cell r="AF16">
-            <v>-34569.5386601153</v>
-          </cell>
-          <cell r="AG16">
-            <v>-6797.3046769533803</v>
-          </cell>
-          <cell r="AH16">
-            <v>28974.929306208502</v>
-          </cell>
-          <cell r="AI16">
-            <v>72747.163289370495</v>
-          </cell>
-          <cell r="AJ16">
-            <v>124519.39727253201</v>
-          </cell>
-          <cell r="AK16">
-            <v>184291.631255694</v>
-          </cell>
-          <cell r="AL16">
-            <v>252063.865238856</v>
-          </cell>
-          <cell r="AM16">
-            <v>327836.09922201798</v>
-          </cell>
-          <cell r="AN16">
-            <v>411608.33320517902</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="I17">
-            <v>1344489.7012446299</v>
-          </cell>
-          <cell r="J17">
-            <v>1200261.9352277899</v>
-          </cell>
-          <cell r="K17">
-            <v>1064034.1692109499</v>
-          </cell>
-          <cell r="L17">
-            <v>935806.40319411794</v>
-          </cell>
-          <cell r="M17">
-            <v>815578.63717728003</v>
-          </cell>
-          <cell r="N17">
-            <v>703350.87116044201</v>
-          </cell>
-          <cell r="O17">
-            <v>599123.10514360399</v>
-          </cell>
-          <cell r="P17">
-            <v>502895.33912676602</v>
-          </cell>
-          <cell r="Q17">
-            <v>414667.57310992799</v>
-          </cell>
-          <cell r="R17">
-            <v>334439.80709309003</v>
-          </cell>
-          <cell r="S17">
-            <v>262212.041076252</v>
-          </cell>
-          <cell r="T17">
-            <v>197984.27505941401</v>
-          </cell>
-          <cell r="U17">
-            <v>141756.50904257601</v>
-          </cell>
-          <cell r="V17">
-            <v>93528.7430257386</v>
-          </cell>
-          <cell r="W17">
-            <v>53300.977008900503</v>
-          </cell>
-          <cell r="X17">
-            <v>21073.210992062501</v>
-          </cell>
-          <cell r="Y17">
-            <v>-3154.55502477549</v>
-          </cell>
-          <cell r="Z17">
-            <v>-19382.321041613501</v>
-          </cell>
-          <cell r="AA17">
-            <v>-27610.0870584515</v>
-          </cell>
-          <cell r="AB17">
-            <v>-27837.8530752896</v>
-          </cell>
-          <cell r="AC17">
-            <v>-20065.619092127599</v>
-          </cell>
-          <cell r="AD17">
-            <v>-4293.38510896568</v>
-          </cell>
-          <cell r="AE17">
-            <v>19478.848874196301</v>
-          </cell>
-          <cell r="AF17">
-            <v>51251.082857358197</v>
-          </cell>
-          <cell r="AG17">
-            <v>91023.316840520201</v>
-          </cell>
-          <cell r="AH17">
-            <v>138795.55082368199</v>
-          </cell>
-          <cell r="AI17">
-            <v>194567.78480684399</v>
-          </cell>
-          <cell r="AJ17">
-            <v>258340.018790006</v>
-          </cell>
-          <cell r="AK17">
-            <v>330112.25277316698</v>
-          </cell>
-          <cell r="AL17">
-            <v>409884.48675632902</v>
-          </cell>
-          <cell r="AM17">
-            <v>497656.72073949099</v>
-          </cell>
-          <cell r="AN17">
-            <v>593428.95472265303</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="I18">
-            <v>1154310.3227621</v>
-          </cell>
-          <cell r="J18">
-            <v>1022082.55674526</v>
-          </cell>
-          <cell r="K18">
-            <v>897854.79072843003</v>
-          </cell>
-          <cell r="L18">
-            <v>781627.02471159201</v>
-          </cell>
-          <cell r="M18">
-            <v>673399.25869475398</v>
-          </cell>
-          <cell r="N18">
-            <v>573171.49267791596</v>
-          </cell>
-          <cell r="O18">
-            <v>480943.72666107799</v>
-          </cell>
-          <cell r="P18">
-            <v>396715.96064424003</v>
-          </cell>
-          <cell r="Q18">
-            <v>320488.194627402</v>
-          </cell>
-          <cell r="R18">
-            <v>252260.42861056401</v>
-          </cell>
-          <cell r="S18">
-            <v>192032.66259372601</v>
-          </cell>
-          <cell r="T18">
-            <v>139804.89657688799</v>
-          </cell>
-          <cell r="U18">
-            <v>95577.130560050195</v>
-          </cell>
-          <cell r="V18">
-            <v>59349.364543212199</v>
-          </cell>
-          <cell r="W18">
-            <v>31121.598526374099</v>
-          </cell>
-          <cell r="X18">
-            <v>10893.8325095361</v>
-          </cell>
-          <cell r="Y18">
-            <v>-1333.9335073018899</v>
-          </cell>
-          <cell r="Z18">
-            <v>-5561.69952413993</v>
-          </cell>
-          <cell r="AA18">
-            <v>-1789.46554097796</v>
-          </cell>
-          <cell r="AB18">
-            <v>9982.7684421840004</v>
-          </cell>
-          <cell r="AC18">
-            <v>29755.002425345901</v>
-          </cell>
-          <cell r="AD18">
-            <v>57527.236408507903</v>
-          </cell>
-          <cell r="AE18">
-            <v>93299.470391669805</v>
-          </cell>
-          <cell r="AF18">
-            <v>137071.704374831</v>
-          </cell>
-          <cell r="AG18">
-            <v>188843.938357993</v>
-          </cell>
-          <cell r="AH18">
-            <v>248616.172341155</v>
-          </cell>
-          <cell r="AI18">
-            <v>316388.40632431698</v>
-          </cell>
-          <cell r="AJ18">
-            <v>392160.64030747901</v>
-          </cell>
-          <cell r="AK18">
-            <v>475932.87429064099</v>
-          </cell>
-          <cell r="AL18">
-            <v>567705.10827380302</v>
-          </cell>
-          <cell r="AM18">
-            <v>667477.342256965</v>
-          </cell>
-          <cell r="AN18">
-            <v>775249.57624012697</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="I19">
-            <v>964130.94427957898</v>
-          </cell>
-          <cell r="J19">
-            <v>843903.17826274096</v>
-          </cell>
-          <cell r="K19">
-            <v>731675.41224590305</v>
-          </cell>
-          <cell r="L19">
-            <v>627447.64622906502</v>
-          </cell>
-          <cell r="M19">
-            <v>531219.880212227</v>
-          </cell>
-          <cell r="N19">
-            <v>442992.11419539002</v>
-          </cell>
-          <cell r="O19">
-            <v>362764.348178552</v>
-          </cell>
-          <cell r="P19">
-            <v>290536.58216171397</v>
-          </cell>
-          <cell r="Q19">
-            <v>226308.81614487601</v>
-          </cell>
-          <cell r="R19">
-            <v>170081.05012803699</v>
-          </cell>
-          <cell r="S19">
-            <v>121853.284111199</v>
-          </cell>
-          <cell r="T19">
-            <v>81625.518094361905</v>
-          </cell>
-          <cell r="U19">
-            <v>49397.752077523801</v>
-          </cell>
-          <cell r="V19">
-            <v>25169.986060685798</v>
-          </cell>
-          <cell r="W19">
-            <v>8942.2200438477794</v>
-          </cell>
-          <cell r="X19">
-            <v>714.45402700974603</v>
-          </cell>
-          <cell r="Y19">
-            <v>486.68801017171103</v>
-          </cell>
-          <cell r="Z19">
-            <v>8258.9219933336699</v>
-          </cell>
-          <cell r="AA19">
-            <v>24031.1559764956</v>
-          </cell>
-          <cell r="AB19">
-            <v>47803.389959657601</v>
-          </cell>
-          <cell r="AC19">
-            <v>79575.623942819497</v>
-          </cell>
-          <cell r="AD19">
-            <v>119347.85792598101</v>
-          </cell>
-          <cell r="AE19">
-            <v>167120.091909143</v>
-          </cell>
-          <cell r="AF19">
-            <v>222892.325892305</v>
-          </cell>
-          <cell r="AG19">
-            <v>286664.55987546698</v>
-          </cell>
-          <cell r="AH19">
-            <v>358436.79385862901</v>
-          </cell>
-          <cell r="AI19">
-            <v>438209.02784179099</v>
-          </cell>
-          <cell r="AJ19">
-            <v>525981.26182495302</v>
-          </cell>
-          <cell r="AK19">
-            <v>621753.495808115</v>
-          </cell>
-          <cell r="AL19">
-            <v>725525.72979127604</v>
-          </cell>
-          <cell r="AM19">
-            <v>837297.96377443802</v>
-          </cell>
-          <cell r="AN19">
-            <v>957070.19775759999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="I20">
-            <v>773951.56579705304</v>
-          </cell>
-          <cell r="J20">
-            <v>665723.79978021502</v>
-          </cell>
-          <cell r="K20">
-            <v>565496.033763377</v>
-          </cell>
-          <cell r="L20">
-            <v>473268.26774653897</v>
-          </cell>
-          <cell r="M20">
-            <v>389040.50172970101</v>
-          </cell>
-          <cell r="N20">
-            <v>312812.73571286298</v>
-          </cell>
-          <cell r="O20">
-            <v>244584.96969602499</v>
-          </cell>
-          <cell r="P20">
-            <v>184357.20367918699</v>
-          </cell>
-          <cell r="Q20">
-            <v>132129.437662349</v>
-          </cell>
-          <cell r="R20">
-            <v>87901.671645511495</v>
-          </cell>
-          <cell r="S20">
-            <v>51673.905628673499</v>
-          </cell>
-          <cell r="T20">
-            <v>23446.139611835501</v>
-          </cell>
-          <cell r="U20">
-            <v>3218.3735949974698</v>
-          </cell>
-          <cell r="V20">
-            <v>-9009.3924218405591</v>
-          </cell>
-          <cell r="W20">
-            <v>-13237.1584386786</v>
-          </cell>
-          <cell r="X20">
-            <v>-9464.9244555166406</v>
-          </cell>
-          <cell r="Y20">
-            <v>2307.30952764531</v>
-          </cell>
-          <cell r="Z20">
-            <v>22079.543510807202</v>
-          </cell>
-          <cell r="AA20">
-            <v>49851.777493969203</v>
-          </cell>
-          <cell r="AB20">
-            <v>85624.011477131193</v>
-          </cell>
-          <cell r="AC20">
-            <v>129396.24546029299</v>
-          </cell>
-          <cell r="AD20">
-            <v>181168.479443455</v>
-          </cell>
-          <cell r="AE20">
-            <v>240940.713426617</v>
-          </cell>
-          <cell r="AF20">
-            <v>308712.94740977901</v>
-          </cell>
-          <cell r="AG20">
-            <v>384485.18139294098</v>
-          </cell>
-          <cell r="AH20">
-            <v>468257.41537610203</v>
-          </cell>
-          <cell r="AI20">
-            <v>560029.64935926395</v>
-          </cell>
-          <cell r="AJ20">
-            <v>659801.88334242604</v>
-          </cell>
-          <cell r="AK20">
-            <v>767574.11732558801</v>
-          </cell>
-          <cell r="AL20">
-            <v>883346.35130874999</v>
-          </cell>
-          <cell r="AM20">
-            <v>1007118.58529191</v>
-          </cell>
-          <cell r="AN20">
-            <v>1138890.81927507</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="I21">
-            <v>583772.18731452699</v>
-          </cell>
-          <cell r="J21">
-            <v>487544.42129768903</v>
-          </cell>
-          <cell r="K21">
-            <v>399316.655280851</v>
-          </cell>
-          <cell r="L21">
-            <v>319088.88926401298</v>
-          </cell>
-          <cell r="M21">
-            <v>246861.12324717501</v>
-          </cell>
-          <cell r="N21">
-            <v>182633.35723033699</v>
-          </cell>
-          <cell r="O21">
-            <v>126405.59121349901</v>
-          </cell>
-          <cell r="P21">
-            <v>78177.825196661201</v>
-          </cell>
-          <cell r="Q21">
-            <v>37950.059179823198</v>
-          </cell>
-          <cell r="R21">
-            <v>5722.2931629851801</v>
-          </cell>
-          <cell r="S21">
-            <v>-18505.4728538528</v>
-          </cell>
-          <cell r="T21">
-            <v>-34733.238870690897</v>
-          </cell>
-          <cell r="U21">
-            <v>-42961.004887528899</v>
-          </cell>
-          <cell r="V21">
-            <v>-43188.770904366902</v>
-          </cell>
-          <cell r="W21">
-            <v>-35416.536921204999</v>
-          </cell>
-          <cell r="X21">
-            <v>-19644.302938043002</v>
-          </cell>
-          <cell r="Y21">
-            <v>4127.9310451189203</v>
-          </cell>
-          <cell r="Z21">
-            <v>35900.165028280797</v>
-          </cell>
-          <cell r="AA21">
-            <v>75672.399011442802</v>
-          </cell>
-          <cell r="AB21">
-            <v>123444.63299460401</v>
-          </cell>
-          <cell r="AC21">
-            <v>179216.86697776601</v>
-          </cell>
-          <cell r="AD21">
-            <v>242989.10096092799</v>
-          </cell>
-          <cell r="AE21">
-            <v>314761.33494408999</v>
-          </cell>
-          <cell r="AF21">
-            <v>394533.56892725202</v>
-          </cell>
-          <cell r="AG21">
-            <v>482305.802910414</v>
-          </cell>
-          <cell r="AH21">
-            <v>578078.03689357603</v>
-          </cell>
-          <cell r="AI21">
-            <v>681850.27087673801</v>
-          </cell>
-          <cell r="AJ21">
-            <v>793622.50485989999</v>
-          </cell>
-          <cell r="AK21">
-            <v>913394.73884306196</v>
-          </cell>
-          <cell r="AL21">
-            <v>1041166.97282622</v>
-          </cell>
-          <cell r="AM21">
-            <v>1176939.2068093801</v>
-          </cell>
-          <cell r="AN21">
-            <v>1320711.4407925401</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="I22">
-            <v>393592.80883200001</v>
-          </cell>
-          <cell r="J22">
-            <v>309365.04281516199</v>
-          </cell>
-          <cell r="K22">
-            <v>233137.27679832399</v>
-          </cell>
-          <cell r="L22">
-            <v>164909.51078148599</v>
-          </cell>
-          <cell r="M22">
-            <v>104681.744764648</v>
-          </cell>
-          <cell r="N22">
-            <v>52453.978747810899</v>
-          </cell>
-          <cell r="O22">
-            <v>8226.2127309728803</v>
-          </cell>
-          <cell r="P22">
-            <v>-28001.553285865099</v>
-          </cell>
-          <cell r="Q22">
-            <v>-56229.319302703101</v>
-          </cell>
-          <cell r="R22">
-            <v>-76457.085319541206</v>
-          </cell>
-          <cell r="S22">
-            <v>-88684.851336379201</v>
-          </cell>
-          <cell r="T22">
-            <v>-92912.617353217298</v>
-          </cell>
-          <cell r="U22">
-            <v>-89140.383370055293</v>
-          </cell>
-          <cell r="V22">
-            <v>-77368.149386893303</v>
-          </cell>
-          <cell r="W22">
-            <v>-57595.915403731298</v>
-          </cell>
-          <cell r="X22">
-            <v>-29823.681420569399</v>
-          </cell>
-          <cell r="Y22">
-            <v>5948.5525625925202</v>
-          </cell>
-          <cell r="Z22">
-            <v>49720.786545754403</v>
-          </cell>
-          <cell r="AA22">
-            <v>101493.02052891599</v>
-          </cell>
-          <cell r="AB22">
-            <v>161265.25451207801</v>
-          </cell>
-          <cell r="AC22">
-            <v>229037.48849523999</v>
-          </cell>
-          <cell r="AD22">
-            <v>304809.72247840202</v>
-          </cell>
-          <cell r="AE22">
-            <v>388581.956461564</v>
-          </cell>
-          <cell r="AF22">
-            <v>480354.19044472597</v>
-          </cell>
-          <cell r="AG22">
-            <v>580126.42442788801</v>
-          </cell>
-          <cell r="AH22">
-            <v>687898.65841104998</v>
-          </cell>
-          <cell r="AI22">
-            <v>803670.89239421196</v>
-          </cell>
-          <cell r="AJ22">
-            <v>927443.126377373</v>
-          </cell>
-          <cell r="AK22">
-            <v>1059215.36036053</v>
-          </cell>
-          <cell r="AL22">
-            <v>1198987.59434369</v>
-          </cell>
-          <cell r="AM22">
-            <v>1346759.82832685</v>
-          </cell>
-          <cell r="AN22">
-            <v>1502532.06231002</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="I23">
-            <v>203413.43034947399</v>
-          </cell>
-          <cell r="J23">
-            <v>131185.66433263599</v>
-          </cell>
-          <cell r="K23">
-            <v>66957.898315798506</v>
-          </cell>
-          <cell r="L23">
-            <v>10730.1322989603</v>
-          </cell>
-          <cell r="M23">
-            <v>-37497.633717877499</v>
-          </cell>
-          <cell r="N23">
-            <v>-77725.399734715305</v>
-          </cell>
-          <cell r="O23">
-            <v>-109953.165751553</v>
-          </cell>
-          <cell r="P23">
-            <v>-134180.93176839099</v>
-          </cell>
-          <cell r="Q23">
-            <v>-150408.69778522899</v>
-          </cell>
-          <cell r="R23">
-            <v>-158636.46380206701</v>
-          </cell>
-          <cell r="S23">
-            <v>-158864.22981890501</v>
-          </cell>
-          <cell r="T23">
-            <v>-151091.995835743</v>
-          </cell>
-          <cell r="U23">
-            <v>-135319.761852581</v>
-          </cell>
-          <cell r="V23">
-            <v>-111547.52786941901</v>
-          </cell>
-          <cell r="W23">
-            <v>-79775.293886257699</v>
-          </cell>
-          <cell r="X23">
-            <v>-40003.059903095796</v>
-          </cell>
-          <cell r="Y23">
-            <v>7769.17408006613</v>
-          </cell>
-          <cell r="Z23">
-            <v>63541.408063228002</v>
-          </cell>
-          <cell r="AA23">
-            <v>127313.64204639</v>
-          </cell>
-          <cell r="AB23">
-            <v>199085.87602955199</v>
-          </cell>
-          <cell r="AC23">
-            <v>278858.11001271399</v>
-          </cell>
-          <cell r="AD23">
-            <v>366630.34399587498</v>
-          </cell>
-          <cell r="AE23">
-            <v>462402.57797903701</v>
-          </cell>
-          <cell r="AF23">
-            <v>566174.81196219905</v>
-          </cell>
-          <cell r="AG23">
-            <v>677947.04594536102</v>
-          </cell>
-          <cell r="AH23">
-            <v>797719.279928523</v>
-          </cell>
-          <cell r="AI23">
-            <v>925491.51391168498</v>
-          </cell>
-          <cell r="AJ23">
-            <v>1061263.7478948401</v>
-          </cell>
-          <cell r="AK23">
-            <v>1205035.9818780001</v>
-          </cell>
-          <cell r="AL23">
-            <v>1356808.2158611701</v>
-          </cell>
-          <cell r="AM23">
-            <v>1516580.4498443301</v>
-          </cell>
-          <cell r="AN23">
-            <v>1684352.6838274901</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="I24">
-            <v>13234.051866948001</v>
-          </cell>
-          <cell r="J24">
-            <v>-46993.714149889704</v>
-          </cell>
-          <cell r="K24">
-            <v>-99221.480166727895</v>
-          </cell>
-          <cell r="L24">
-            <v>-143449.246183565</v>
-          </cell>
-          <cell r="M24">
-            <v>-179677.012200403</v>
-          </cell>
-          <cell r="N24">
-            <v>-207904.77821724099</v>
-          </cell>
-          <cell r="O24">
-            <v>-228132.54423407899</v>
-          </cell>
-          <cell r="P24">
-            <v>-240360.31025091701</v>
-          </cell>
-          <cell r="Q24">
-            <v>-244588.07626775501</v>
-          </cell>
-          <cell r="R24">
-            <v>-240815.84228459399</v>
-          </cell>
-          <cell r="S24">
-            <v>-229043.60830143199</v>
-          </cell>
-          <cell r="T24">
-            <v>-209271.37431827001</v>
-          </cell>
-          <cell r="U24">
-            <v>-181499.14033510801</v>
-          </cell>
-          <cell r="V24">
-            <v>-145726.906351946</v>
-          </cell>
-          <cell r="W24">
-            <v>-101954.672368784</v>
-          </cell>
-          <cell r="X24">
-            <v>-50182.438385622198</v>
-          </cell>
-          <cell r="Y24">
-            <v>9589.7955975397399</v>
-          </cell>
-          <cell r="Z24">
-            <v>77362.029580701696</v>
-          </cell>
-          <cell r="AA24">
-            <v>153134.263563863</v>
-          </cell>
-          <cell r="AB24">
-            <v>236906.49754702501</v>
-          </cell>
-          <cell r="AC24">
-            <v>328678.73153018701</v>
-          </cell>
-          <cell r="AD24">
-            <v>428450.96551334899</v>
-          </cell>
-          <cell r="AE24">
-            <v>536223.19949651102</v>
-          </cell>
-          <cell r="AF24">
-            <v>651995.433479673</v>
-          </cell>
-          <cell r="AG24">
-            <v>775767.66746283497</v>
-          </cell>
-          <cell r="AH24">
-            <v>907539.90144599695</v>
-          </cell>
-          <cell r="AI24">
-            <v>1047312.13542915</v>
-          </cell>
-          <cell r="AJ24">
-            <v>1195084.36941232</v>
-          </cell>
-          <cell r="AK24">
-            <v>1350856.60339548</v>
-          </cell>
-          <cell r="AL24">
-            <v>1514628.83737864</v>
-          </cell>
-          <cell r="AM24">
-            <v>1686401.0713618</v>
-          </cell>
-          <cell r="AN24">
-            <v>1866173.30534496</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="I25">
-            <v>-176945.326615578</v>
-          </cell>
-          <cell r="J25">
-            <v>-225173.092632416</v>
-          </cell>
-          <cell r="K25">
-            <v>-265400.85864925402</v>
-          </cell>
-          <cell r="L25">
-            <v>-297628.62466609199</v>
-          </cell>
-          <cell r="M25">
-            <v>-321856.39068293001</v>
-          </cell>
-          <cell r="N25">
-            <v>-338084.15669976798</v>
-          </cell>
-          <cell r="O25">
-            <v>-346311.922716606</v>
-          </cell>
-          <cell r="P25">
-            <v>-346539.68873344403</v>
-          </cell>
-          <cell r="Q25">
-            <v>-338767.45475028199</v>
-          </cell>
-          <cell r="R25">
-            <v>-322995.22076712002</v>
-          </cell>
-          <cell r="S25">
-            <v>-299222.98678395798</v>
-          </cell>
-          <cell r="T25">
-            <v>-267450.75280079601</v>
-          </cell>
-          <cell r="U25">
-            <v>-227678.518817634</v>
-          </cell>
-          <cell r="V25">
-            <v>-179906.284834472</v>
-          </cell>
-          <cell r="W25">
-            <v>-124134.05085131001</v>
-          </cell>
-          <cell r="X25">
-            <v>-60361.816868148599</v>
-          </cell>
-          <cell r="Y25">
-            <v>11410.417115013301</v>
-          </cell>
-          <cell r="Z25">
-            <v>91182.651098175294</v>
-          </cell>
-          <cell r="AA25">
-            <v>178954.88508133701</v>
-          </cell>
-          <cell r="AB25">
-            <v>274727.11906449898</v>
-          </cell>
-          <cell r="AC25">
-            <v>378499.35304766102</v>
-          </cell>
-          <cell r="AD25">
-            <v>490271.58703082299</v>
-          </cell>
-          <cell r="AE25">
-            <v>610043.82101398497</v>
-          </cell>
-          <cell r="AF25">
-            <v>737816.05499714694</v>
-          </cell>
-          <cell r="AG25">
-            <v>873588.28898030904</v>
-          </cell>
-          <cell r="AH25">
-            <v>1017360.52296347</v>
-          </cell>
-          <cell r="AI25">
-            <v>1169132.7569466301</v>
-          </cell>
-          <cell r="AJ25">
-            <v>1328904.9909297901</v>
-          </cell>
-          <cell r="AK25">
-            <v>1496677.2249129501</v>
-          </cell>
-          <cell r="AL25">
-            <v>1672449.4588961101</v>
-          </cell>
-          <cell r="AM25">
-            <v>1856221.6928792801</v>
-          </cell>
-          <cell r="AN25">
-            <v>2047993.9268624401</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="I26">
-            <v>-367124.70509810402</v>
-          </cell>
-          <cell r="J26">
-            <v>-403352.47111494199</v>
-          </cell>
-          <cell r="K26">
-            <v>-431580.23713178001</v>
-          </cell>
-          <cell r="L26">
-            <v>-451808.00314861798</v>
-          </cell>
-          <cell r="M26">
-            <v>-464035.769165456</v>
-          </cell>
-          <cell r="N26">
-            <v>-468263.53518229403</v>
-          </cell>
-          <cell r="O26">
-            <v>-464491.30119913199</v>
-          </cell>
-          <cell r="P26">
-            <v>-452719.06721597002</v>
-          </cell>
-          <cell r="Q26">
-            <v>-432946.83323280799</v>
-          </cell>
-          <cell r="R26">
-            <v>-405174.59924964601</v>
-          </cell>
-          <cell r="S26">
-            <v>-369402.36526648398</v>
-          </cell>
-          <cell r="T26">
-            <v>-325630.131283322</v>
-          </cell>
-          <cell r="U26">
-            <v>-273857.89730016002</v>
-          </cell>
-          <cell r="V26">
-            <v>-214085.66331699799</v>
-          </cell>
-          <cell r="W26">
-            <v>-146313.429333837</v>
-          </cell>
-          <cell r="X26">
-            <v>-70541.195350675</v>
-          </cell>
-          <cell r="Y26">
-            <v>13231.0386324869</v>
-          </cell>
-          <cell r="Z26">
-            <v>105003.27261564801</v>
-          </cell>
-          <cell r="AA26">
-            <v>204775.50659881</v>
-          </cell>
-          <cell r="AB26">
-            <v>312547.740581972</v>
-          </cell>
-          <cell r="AC26">
-            <v>428319.97456513398</v>
-          </cell>
-          <cell r="AD26">
-            <v>552092.20854829601</v>
-          </cell>
-          <cell r="AE26">
-            <v>683864.44253145799</v>
-          </cell>
-          <cell r="AF26">
-            <v>823636.67651461996</v>
-          </cell>
-          <cell r="AG26">
-            <v>971408.91049778205</v>
-          </cell>
-          <cell r="AH26">
-            <v>1127181.14448094</v>
-          </cell>
-          <cell r="AI26">
-            <v>1290953.3784641</v>
-          </cell>
-          <cell r="AJ26">
-            <v>1462725.6124472599</v>
-          </cell>
-          <cell r="AK26">
-            <v>1642497.84643043</v>
-          </cell>
-          <cell r="AL26">
-            <v>1830270.08041359</v>
-          </cell>
-          <cell r="AM26">
-            <v>2026042.3143967499</v>
-          </cell>
-          <cell r="AN26">
-            <v>2229814.5483799102</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="I27">
-            <v>-557304.08358063095</v>
-          </cell>
-          <cell r="J27">
-            <v>-581531.84959746897</v>
-          </cell>
-          <cell r="K27">
-            <v>-597759.615614307</v>
-          </cell>
-          <cell r="L27">
-            <v>-605987.38163114502</v>
-          </cell>
-          <cell r="M27">
-            <v>-606215.14764798305</v>
-          </cell>
-          <cell r="N27">
-            <v>-598442.91366482095</v>
-          </cell>
-          <cell r="O27">
-            <v>-582670.67968165898</v>
-          </cell>
-          <cell r="P27">
-            <v>-558898.445698497</v>
-          </cell>
-          <cell r="Q27">
-            <v>-527126.21171533503</v>
-          </cell>
-          <cell r="R27">
-            <v>-487353.97773217299</v>
-          </cell>
-          <cell r="S27">
-            <v>-439581.74374901102</v>
-          </cell>
-          <cell r="T27">
-            <v>-383809.50976584898</v>
-          </cell>
-          <cell r="U27">
-            <v>-320037.27578268701</v>
-          </cell>
-          <cell r="V27">
-            <v>-248265.041799525</v>
-          </cell>
-          <cell r="W27">
-            <v>-168492.807816363</v>
-          </cell>
-          <cell r="X27">
-            <v>-80720.573833201401</v>
-          </cell>
-          <cell r="Y27">
-            <v>15051.6601499605</v>
-          </cell>
-          <cell r="Z27">
-            <v>118823.894133122</v>
-          </cell>
-          <cell r="AA27">
-            <v>230596.128116284</v>
-          </cell>
-          <cell r="AB27">
-            <v>350368.36209944601</v>
-          </cell>
-          <cell r="AC27">
-            <v>478140.59608260798</v>
-          </cell>
-          <cell r="AD27">
-            <v>613912.83006576996</v>
-          </cell>
-          <cell r="AE27">
-            <v>757685.06404893205</v>
-          </cell>
-          <cell r="AF27">
-            <v>909457.29803209403</v>
-          </cell>
-          <cell r="AG27">
-            <v>1069229.5320152501</v>
-          </cell>
-          <cell r="AH27">
-            <v>1237001.7659984101</v>
-          </cell>
-          <cell r="AI27">
-            <v>1412773.9999815701</v>
-          </cell>
-          <cell r="AJ27">
-            <v>1596546.2339647401</v>
-          </cell>
-          <cell r="AK27">
-            <v>1788318.4679479001</v>
-          </cell>
-          <cell r="AL27">
-            <v>1988090.7019310601</v>
-          </cell>
-          <cell r="AM27">
-            <v>2195862.9359142198</v>
-          </cell>
-          <cell r="AN27">
-            <v>2411635.1698973798</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="I28">
-            <v>-747483.462063157</v>
-          </cell>
-          <cell r="J28">
-            <v>-759711.22807999398</v>
-          </cell>
-          <cell r="K28">
-            <v>-763938.99409683305</v>
-          </cell>
-          <cell r="L28">
-            <v>-760166.76011367096</v>
-          </cell>
-          <cell r="M28">
-            <v>-748394.52613050898</v>
-          </cell>
-          <cell r="N28">
-            <v>-728622.29214734701</v>
-          </cell>
-          <cell r="O28">
-            <v>-700850.05816418503</v>
-          </cell>
-          <cell r="P28">
-            <v>-665077.82418102305</v>
-          </cell>
-          <cell r="Q28">
-            <v>-621305.59019786096</v>
-          </cell>
-          <cell r="R28">
-            <v>-569533.35621469899</v>
-          </cell>
-          <cell r="S28">
-            <v>-509761.12223153701</v>
-          </cell>
-          <cell r="T28">
-            <v>-441988.88824837498</v>
-          </cell>
-          <cell r="U28">
-            <v>-366216.654265213</v>
-          </cell>
-          <cell r="V28">
-            <v>-282444.42028205103</v>
-          </cell>
-          <cell r="W28">
-            <v>-190672.18629888899</v>
-          </cell>
-          <cell r="X28">
-            <v>-90899.9523157277</v>
-          </cell>
-          <cell r="Y28">
-            <v>16872.281667434101</v>
-          </cell>
-          <cell r="Z28">
-            <v>132644.515650596</v>
-          </cell>
-          <cell r="AA28">
-            <v>256416.74963375801</v>
-          </cell>
-          <cell r="AB28">
-            <v>388188.98361692001</v>
-          </cell>
-          <cell r="AC28">
-            <v>527961.217600081</v>
-          </cell>
-          <cell r="AD28">
-            <v>675733.45158324298</v>
-          </cell>
-          <cell r="AE28">
-            <v>831505.68556640495</v>
-          </cell>
-          <cell r="AF28">
-            <v>995277.91954956704</v>
-          </cell>
-          <cell r="AG28">
-            <v>1167050.1535327299</v>
-          </cell>
-          <cell r="AH28">
-            <v>1346822.3875158899</v>
-          </cell>
-          <cell r="AI28">
-            <v>1534594.6214990499</v>
-          </cell>
-          <cell r="AJ28">
-            <v>1730366.8554822099</v>
-          </cell>
-          <cell r="AK28">
-            <v>1934139.0894653699</v>
-          </cell>
-          <cell r="AL28">
-            <v>2145911.3234485299</v>
-          </cell>
-          <cell r="AM28">
-            <v>2365683.5574317002</v>
-          </cell>
-          <cell r="AN28">
-            <v>2593455.7914148602</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="I29">
-            <v>-937662.84054568305</v>
-          </cell>
-          <cell r="J29">
-            <v>-937890.60656252096</v>
-          </cell>
-          <cell r="K29">
-            <v>-930118.37257935898</v>
-          </cell>
-          <cell r="L29">
-            <v>-914346.13859619701</v>
-          </cell>
-          <cell r="M29">
-            <v>-890573.90461303503</v>
-          </cell>
-          <cell r="N29">
-            <v>-858801.67062987306</v>
-          </cell>
-          <cell r="O29">
-            <v>-819029.43664671096</v>
-          </cell>
-          <cell r="P29">
-            <v>-771257.20266354899</v>
-          </cell>
-          <cell r="Q29">
-            <v>-715484.96868038701</v>
-          </cell>
-          <cell r="R29">
-            <v>-651712.73469722597</v>
-          </cell>
-          <cell r="S29">
-            <v>-579940.50071406399</v>
-          </cell>
-          <cell r="T29">
-            <v>-500168.26673090202</v>
-          </cell>
-          <cell r="U29">
-            <v>-412396.03274773998</v>
-          </cell>
-          <cell r="V29">
-            <v>-316623.79876457801</v>
-          </cell>
-          <cell r="W29">
-            <v>-212851.564781416</v>
-          </cell>
-          <cell r="X29">
-            <v>-101079.330798254</v>
-          </cell>
-          <cell r="Y29">
-            <v>18692.9031849077</v>
-          </cell>
-          <cell r="Z29">
-            <v>146465.13716806899</v>
-          </cell>
-          <cell r="AA29">
-            <v>282237.371151231</v>
-          </cell>
-          <cell r="AB29">
-            <v>426009.60513439297</v>
-          </cell>
-          <cell r="AC29">
-            <v>577781.83911755495</v>
-          </cell>
-          <cell r="AD29">
-            <v>737554.07310071704</v>
-          </cell>
-          <cell r="AE29">
-            <v>905326.30708387902</v>
-          </cell>
-          <cell r="AF29">
-            <v>1081098.5410670401</v>
-          </cell>
-          <cell r="AG29">
-            <v>1264870.7750502001</v>
-          </cell>
-          <cell r="AH29">
-            <v>1456643.0090333601</v>
-          </cell>
-          <cell r="AI29">
-            <v>1656415.24301652</v>
-          </cell>
-          <cell r="AJ29">
-            <v>1864187.47699968</v>
-          </cell>
-          <cell r="AK29">
-            <v>2079959.7109828501</v>
-          </cell>
-          <cell r="AL29">
-            <v>2303731.9449660098</v>
-          </cell>
-          <cell r="AM29">
-            <v>2535504.1789491698</v>
-          </cell>
-          <cell r="AN29">
-            <v>2775276.4129323298</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="I30">
-            <v>-1127842.2190282</v>
-          </cell>
-          <cell r="J30">
-            <v>-1116069.98504504</v>
-          </cell>
-          <cell r="K30">
-            <v>-1096297.75106188</v>
-          </cell>
-          <cell r="L30">
-            <v>-1068525.51707872</v>
-          </cell>
-          <cell r="M30">
-            <v>-1032753.28309556</v>
-          </cell>
-          <cell r="N30">
-            <v>-988981.04911239899</v>
-          </cell>
-          <cell r="O30">
-            <v>-937208.81512923702</v>
-          </cell>
-          <cell r="P30">
-            <v>-877436.58114607597</v>
-          </cell>
-          <cell r="Q30">
-            <v>-809664.347162914</v>
-          </cell>
-          <cell r="R30">
-            <v>-733892.11317975202</v>
-          </cell>
-          <cell r="S30">
-            <v>-650119.87919659005</v>
-          </cell>
-          <cell r="T30">
-            <v>-558347.64521342795</v>
-          </cell>
-          <cell r="U30">
-            <v>-458575.41123026598</v>
-          </cell>
-          <cell r="V30">
-            <v>-350803.177247104</v>
-          </cell>
-          <cell r="W30">
-            <v>-235030.943263942</v>
-          </cell>
-          <cell r="X30">
-            <v>-111258.70928078001</v>
-          </cell>
-          <cell r="Y30">
-            <v>20513.524702381299</v>
-          </cell>
-          <cell r="Z30">
-            <v>160285.758685543</v>
-          </cell>
-          <cell r="AA30">
-            <v>308057.992668705</v>
-          </cell>
-          <cell r="AB30">
-            <v>463830.22665186698</v>
-          </cell>
-          <cell r="AC30">
-            <v>627602.46063502901</v>
-          </cell>
-          <cell r="AD30">
-            <v>799374.69461819099</v>
-          </cell>
-          <cell r="AE30">
-            <v>979146.92860135203</v>
-          </cell>
-          <cell r="AF30">
-            <v>1166919.1625845099</v>
-          </cell>
-          <cell r="AG30">
-            <v>1362691.3965676699</v>
-          </cell>
-          <cell r="AH30">
-            <v>1566463.6305508299</v>
-          </cell>
-          <cell r="AI30">
-            <v>1778235.8645339999</v>
-          </cell>
-          <cell r="AJ30">
-            <v>1998008.0985171599</v>
-          </cell>
-          <cell r="AK30">
-            <v>2225780.3325003199</v>
-          </cell>
-          <cell r="AL30">
-            <v>2461552.5664834799</v>
-          </cell>
-          <cell r="AM30">
-            <v>2705324.8004666399</v>
-          </cell>
-          <cell r="AN30">
-            <v>2957097.0344497999</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="I31">
-            <v>-1318021.5975107299</v>
-          </cell>
-          <cell r="J31">
-            <v>-1294249.3635275699</v>
-          </cell>
-          <cell r="K31">
-            <v>-1262477.1295444099</v>
-          </cell>
-          <cell r="L31">
-            <v>-1222704.8955612499</v>
-          </cell>
-          <cell r="M31">
-            <v>-1174932.6615780799</v>
-          </cell>
-          <cell r="N31">
-            <v>-1119160.4275949199</v>
-          </cell>
-          <cell r="O31">
-            <v>-1055388.1936117599</v>
-          </cell>
-          <cell r="P31">
-            <v>-983615.95962860202</v>
-          </cell>
-          <cell r="Q31">
-            <v>-903843.72564544005</v>
-          </cell>
-          <cell r="R31">
-            <v>-816071.49166227796</v>
-          </cell>
-          <cell r="S31">
-            <v>-720299.25767911598</v>
-          </cell>
-          <cell r="T31">
-            <v>-616527.02369595401</v>
-          </cell>
-          <cell r="U31">
-            <v>-504754.78971279197</v>
-          </cell>
-          <cell r="V31">
-            <v>-384982.55572963</v>
-          </cell>
-          <cell r="W31">
-            <v>-257210.32174646799</v>
-          </cell>
-          <cell r="X31">
-            <v>-121438.087763306</v>
-          </cell>
-          <cell r="Y31">
-            <v>22334.146219854902</v>
-          </cell>
-          <cell r="Z31">
-            <v>174106.38020301599</v>
-          </cell>
-          <cell r="AA31">
-            <v>333878.61418617802</v>
-          </cell>
-          <cell r="AB31">
-            <v>501650.84816934</v>
-          </cell>
-          <cell r="AC31">
-            <v>677423.08215250203</v>
-          </cell>
-          <cell r="AD31">
-            <v>861195.316135664</v>
-          </cell>
-          <cell r="AE31">
-            <v>1052967.55011882</v>
-          </cell>
-          <cell r="AF31">
-            <v>1252739.78410198</v>
-          </cell>
-          <cell r="AG31">
-            <v>1460512.01808515</v>
-          </cell>
-          <cell r="AH31">
-            <v>1676284.25206831</v>
-          </cell>
-          <cell r="AI31">
-            <v>1900056.48605147</v>
-          </cell>
-          <cell r="AJ31">
-            <v>2131828.72003463</v>
-          </cell>
-          <cell r="AK31">
-            <v>2371600.95401779</v>
-          </cell>
-          <cell r="AL31">
-            <v>2619373.18800095</v>
-          </cell>
-          <cell r="AM31">
-            <v>2875145.4219841198</v>
-          </cell>
-          <cell r="AN31">
-            <v>3138917.6559672798</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="I32">
-            <v>-1508200.97599326</v>
-          </cell>
-          <cell r="J32">
-            <v>-1472428.74201009</v>
-          </cell>
-          <cell r="K32">
-            <v>-1428656.50802693</v>
-          </cell>
-          <cell r="L32">
-            <v>-1376884.27404377</v>
-          </cell>
-          <cell r="M32">
-            <v>-1317112.04006061</v>
-          </cell>
-          <cell r="N32">
-            <v>-1249339.80607745</v>
-          </cell>
-          <cell r="O32">
-            <v>-1173567.5720942901</v>
-          </cell>
-          <cell r="P32">
-            <v>-1089795.33811112</v>
-          </cell>
-          <cell r="Q32">
-            <v>-998023.10412796598</v>
-          </cell>
-          <cell r="R32">
-            <v>-898250.87014480506</v>
-          </cell>
-          <cell r="S32">
-            <v>-790478.63616164296</v>
-          </cell>
-          <cell r="T32">
-            <v>-674706.40217848099</v>
-          </cell>
-          <cell r="U32">
-            <v>-550934.16819531901</v>
-          </cell>
-          <cell r="V32">
-            <v>-419161.93421215698</v>
-          </cell>
-          <cell r="W32">
-            <v>-279389.700228995</v>
-          </cell>
-          <cell r="X32">
-            <v>-131617.466245833</v>
-          </cell>
-          <cell r="Y32">
-            <v>24154.767737328501</v>
-          </cell>
-          <cell r="Z32">
-            <v>187927.00172048999</v>
-          </cell>
-          <cell r="AA32">
-            <v>359699.23570365203</v>
-          </cell>
-          <cell r="AB32">
-            <v>539471.469686814</v>
-          </cell>
-          <cell r="AC32">
-            <v>727243.70366997598</v>
-          </cell>
-          <cell r="AD32">
-            <v>923015.93765313795</v>
-          </cell>
-          <cell r="AE32">
-            <v>1126788.1716362999</v>
-          </cell>
-          <cell r="AF32">
-            <v>1338560.4056194599</v>
-          </cell>
-          <cell r="AG32">
-            <v>1558332.6396026199</v>
-          </cell>
-          <cell r="AH32">
-            <v>1786104.8735857799</v>
-          </cell>
-          <cell r="AI32">
-            <v>2021877.1075689399</v>
-          </cell>
-          <cell r="AJ32">
-            <v>2265649.3415521001</v>
-          </cell>
-          <cell r="AK32">
-            <v>2517421.5755352699</v>
-          </cell>
-          <cell r="AL32">
-            <v>2777193.8095184299</v>
-          </cell>
-          <cell r="AM32">
-            <v>3044966.0435015899</v>
-          </cell>
-          <cell r="AN32">
-            <v>3320738.2774847499</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="I33">
-            <v>-1698380.3544757799</v>
-          </cell>
-          <cell r="J33">
-            <v>-1650608.1204926199</v>
-          </cell>
-          <cell r="K33">
-            <v>-1594835.8865094599</v>
-          </cell>
-          <cell r="L33">
-            <v>-1531063.6525262999</v>
-          </cell>
-          <cell r="M33">
-            <v>-1459291.4185431399</v>
-          </cell>
-          <cell r="N33">
-            <v>-1379519.1845599699</v>
-          </cell>
-          <cell r="O33">
-            <v>-1291746.9505768099</v>
-          </cell>
-          <cell r="P33">
-            <v>-1195974.7165936499</v>
-          </cell>
-          <cell r="Q33">
-            <v>-1092202.4826104899</v>
-          </cell>
-          <cell r="R33">
-            <v>-980430.24862733099</v>
-          </cell>
-          <cell r="S33">
-            <v>-860658.01464416902</v>
-          </cell>
-          <cell r="T33">
-            <v>-732885.78066100704</v>
-          </cell>
-          <cell r="U33">
-            <v>-597113.54667784495</v>
-          </cell>
-          <cell r="V33">
-            <v>-453341.31269468297</v>
-          </cell>
-          <cell r="W33">
-            <v>-301569.078711521</v>
-          </cell>
-          <cell r="X33">
-            <v>-141796.84472835899</v>
-          </cell>
-          <cell r="Y33">
-            <v>25975.389254802099</v>
-          </cell>
-          <cell r="Z33">
-            <v>201747.623237964</v>
-          </cell>
-          <cell r="AA33">
-            <v>385519.85722112597</v>
-          </cell>
-          <cell r="AB33">
-            <v>577292.09120428702</v>
-          </cell>
-          <cell r="AC33">
-            <v>777064.32518744899</v>
-          </cell>
-          <cell r="AD33">
-            <v>984836.55917061097</v>
-          </cell>
-          <cell r="AE33">
-            <v>1200608.79315377</v>
-          </cell>
-          <cell r="AF33">
-            <v>1424381.02713693</v>
-          </cell>
-          <cell r="AG33">
-            <v>1656153.26112009</v>
-          </cell>
-          <cell r="AH33">
-            <v>1895925.49510325</v>
-          </cell>
-          <cell r="AI33">
-            <v>2143697.72908642</v>
-          </cell>
-          <cell r="AJ33">
-            <v>2399469.96306958</v>
-          </cell>
-          <cell r="AK33">
-            <v>2663242.19705274</v>
-          </cell>
-          <cell r="AL33">
-            <v>2935014.4310359</v>
-          </cell>
-          <cell r="AM33">
-            <v>3214786.66501906</v>
-          </cell>
-          <cell r="AN33">
-            <v>3502558.89900222</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="I34">
-            <v>-1888559.7329583101</v>
-          </cell>
-          <cell r="J34">
-            <v>-1828787.4989751501</v>
-          </cell>
-          <cell r="K34">
-            <v>-1761015.2649919901</v>
-          </cell>
-          <cell r="L34">
-            <v>-1685243.03100882</v>
-          </cell>
-          <cell r="M34">
-            <v>-1601470.7970256601</v>
-          </cell>
-          <cell r="N34">
-            <v>-1509698.5630425001</v>
-          </cell>
-          <cell r="O34">
-            <v>-1409926.3290593401</v>
-          </cell>
-          <cell r="P34">
-            <v>-1302154.0950761801</v>
-          </cell>
-          <cell r="Q34">
-            <v>-1186381.8610930101</v>
-          </cell>
-          <cell r="R34">
-            <v>-1062609.6271098501</v>
-          </cell>
-          <cell r="S34">
-            <v>-930837.39312669495</v>
-          </cell>
-          <cell r="T34">
-            <v>-791065.15914353298</v>
-          </cell>
-          <cell r="U34">
-            <v>-643292.925160371</v>
-          </cell>
-          <cell r="V34">
-            <v>-487520.69117720902</v>
-          </cell>
-          <cell r="W34">
-            <v>-323748.45719404798</v>
-          </cell>
-          <cell r="X34">
-            <v>-151976.223210886</v>
-          </cell>
-          <cell r="Y34">
-            <v>27796.010772275698</v>
-          </cell>
-          <cell r="Z34">
-            <v>215568.24475543699</v>
-          </cell>
-          <cell r="AA34">
-            <v>411340.47873859899</v>
-          </cell>
-          <cell r="AB34">
-            <v>615112.71272176097</v>
-          </cell>
-          <cell r="AC34">
-            <v>826884.94670492294</v>
-          </cell>
-          <cell r="AD34">
-            <v>1046657.18068808</v>
-          </cell>
-          <cell r="AE34">
-            <v>1274429.4146712399</v>
-          </cell>
-          <cell r="AF34">
-            <v>1510201.6486543999</v>
-          </cell>
-          <cell r="AG34">
-            <v>1753973.8826375699</v>
-          </cell>
-          <cell r="AH34">
-            <v>2005746.1166207299</v>
-          </cell>
-          <cell r="AI34">
-            <v>2265518.3506038901</v>
-          </cell>
-          <cell r="AJ34">
-            <v>2533290.5845870501</v>
-          </cell>
-          <cell r="AK34">
-            <v>2809062.8185702101</v>
-          </cell>
-          <cell r="AL34">
-            <v>3092835.0525533701</v>
-          </cell>
-          <cell r="AM34">
-            <v>3384607.2865365399</v>
-          </cell>
-          <cell r="AN34">
-            <v>3684379.5205196999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -20033,7 +16875,7 @@
   <dimension ref="A1:AN1024"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38:AN70"/>
+      <selection activeCell="H2" sqref="H2:AN70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>